<commit_message>
moved Xbudget lines from Sheet1 to Sheet2 where they will not be used
</commit_message>
<xml_diff>
--- a/input_files/map.xlsx
+++ b/input_files/map.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\01_Dave\Programs\GitHub_home\budget\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BB7802-84F1-4952-AE60-AD9A628606F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFBDF63-9F0C-4264-A3B5-FEF509F8C7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$236</definedName>
-    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable21" hidden="1">'[1]budget 11-01-23'!$A$1:$M$198</definedName>
-    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable31" hidden="1">Table1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$222</definedName>
+    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable2" hidden="1">'[1]budget 11-01-23'!$A$1:$M$198</definedName>
+    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable3" hidden="1">Table1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -120,7 +121,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table2" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable21"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable2"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -129,7 +130,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table3">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable31"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable3"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1267,7 +1268,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6F80153F-CDA1-4E91-9FDD-43E3E0555995}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1502,12 +1510,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M236"/>
+  <dimension ref="A1:M222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L17" sqref="L17"/>
-      <selection pane="bottomLeft" activeCell="D91" sqref="D91:D92"/>
+      <selection pane="bottomLeft" activeCell="A223" sqref="A223:XFD236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10623,522 +10631,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A223" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B223" s="1" t="str">
-        <f>C223</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="C223" s="1" t="str">
-        <f>D223</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F223" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G223" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H223" t="s">
-        <v>250</v>
-      </c>
-      <c r="L223" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M223" s="1">
-        <f>IF(B223=B222,M222,M222+1)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A224" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B224" s="1" t="str">
-        <f>C224</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="C224" s="1" t="str">
-        <f>D224</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="D224" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F224" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G224" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H224" t="s">
-        <v>241</v>
-      </c>
-      <c r="L224" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M224" s="1">
-        <f>IF(B224=B223,M223,M223+1)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A225" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B225" s="1" t="str">
-        <f>C225</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="C225" s="1" t="str">
-        <f>D225</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="D225" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F225" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G225" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H225" t="s">
-        <v>251</v>
-      </c>
-      <c r="L225" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M225" s="1">
-        <f>IF(B225=B224,M224,M224+1)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A226" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B226" s="1" t="str">
-        <f>C226</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="C226" s="1" t="str">
-        <f>D226</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="D226" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F226" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G226" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H226" t="s">
-        <v>252</v>
-      </c>
-      <c r="L226" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M226" s="1">
-        <f>IF(B226=B225,M225,M225+1)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A227" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B227" s="1" t="str">
-        <f>C227</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="C227" s="1" t="str">
-        <f>D227</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="D227" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F227" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G227" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H227" t="s">
-        <v>253</v>
-      </c>
-      <c r="L227" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M227" s="1">
-        <f>IF(B227=B226,M226,M226+1)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A228" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B228" s="1" t="str">
-        <f>C228</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="C228" s="1" t="str">
-        <f>D228</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="D228" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F228" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G228" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H228" t="s">
-        <v>254</v>
-      </c>
-      <c r="L228" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M228" s="1">
-        <f>IF(B228=B227,M227,M227+1)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A229" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B229" s="1" t="str">
-        <f>C229</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="C229" s="1" t="str">
-        <f>D229</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="D229" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F229" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G229" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H229" t="s">
-        <v>255</v>
-      </c>
-      <c r="L229" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M229" s="1">
-        <f>IF(B229=B228,M228,M228+1)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A230" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B230" s="1" t="str">
-        <f>C230</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="C230" s="1" t="str">
-        <f>D230</f>
-        <v>20 Xbudget</v>
-      </c>
-      <c r="D230" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F230" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G230" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H230" t="s">
-        <v>256</v>
-      </c>
-      <c r="L230" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M230" s="1">
-        <f>IF(B230=B229,M229,M229+1)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A231" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B231" s="1" t="str">
-        <f>C231</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="C231" s="1" t="str">
-        <f>D231</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="D231" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F231" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G231" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H231" t="s">
-        <v>244</v>
-      </c>
-      <c r="I231" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="L231" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M231" s="1">
-        <f>IF(B231=B230,M230,M230+1)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A232" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B232" s="1" t="str">
-        <f>C232</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="C232" s="1" t="str">
-        <f>D232</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="D232" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F232" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G232" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H232" t="s">
-        <v>245</v>
-      </c>
-      <c r="I232" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="L232" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M232" s="1">
-        <f>IF(B232=B231,M231,M231+1)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A233" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B233" s="1" t="str">
-        <f>C233</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="C233" s="1" t="str">
-        <f>D233</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="D233" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F233" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G233" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H233" t="s">
-        <v>237</v>
-      </c>
-      <c r="I233" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="L233" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M233" s="1">
-        <f>IF(B233=B232,M232,M232+1)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A234" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B234" s="1" t="str">
-        <f>C234</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="C234" s="1" t="str">
-        <f>D234</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="D234" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F234" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G234" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H234" t="s">
-        <v>238</v>
-      </c>
-      <c r="I234" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="L234" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M234" s="1">
-        <f>IF(B234=B233,M233,M233+1)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A235" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B235" s="1" t="str">
-        <f>C235</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="C235" s="1" t="str">
-        <f>D235</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="D235" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F235" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G235" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H235" t="s">
-        <v>246</v>
-      </c>
-      <c r="I235" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="L235" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M235" s="1">
-        <f>IF(B235=B234,M234,M234+1)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A236" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B236" s="1" t="str">
-        <f>C236</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="C236" s="1" t="str">
-        <f>D236</f>
-        <v>Xbudget</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F236" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G236" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H236" t="s">
-        <v>247</v>
-      </c>
-      <c r="I236" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="L236" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M236" s="1">
-        <f>IF(B236=B235,M235,M235+1)</f>
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:M236" xr:uid="{9210D030-08A6-47C5-BE1B-A368CD904E6C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M236">
       <sortCondition ref="D1:D236"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A2:M236">
-    <cfRule type="expression" dxfId="0" priority="5">
+  <conditionalFormatting sqref="A2:M222">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>MOD($M2,2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11147,4 +10647,532 @@
   <pageSetup scale="40" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6BED37-98F6-447C-9D06-707E3FCDE95E}">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>C1</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f>D1</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H1" t="s">
+        <v>250</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M1" s="1">
+        <f>IF(B1=Sheet1!B222,Sheet1!M222,Sheet1!M222+1)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>C2</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>D2</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H2" t="s">
+        <v>241</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M2" s="1">
+        <f>IF(B2=B1,M1,M1+1)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f>C3</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>D3</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H3" t="s">
+        <v>251</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M3" s="1">
+        <f>IF(B3=B2,M2,M2+1)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>C4</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>D4</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H4" t="s">
+        <v>252</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M4" s="1">
+        <f>IF(B4=B3,M3,M3+1)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f>C5</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>D5</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H5" t="s">
+        <v>253</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M5" s="1">
+        <f>IF(B5=B4,M4,M4+1)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f>C6</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f>D6</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H6" t="s">
+        <v>254</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M6" s="1">
+        <f>IF(B6=B5,M5,M5+1)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f>C7</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f>D7</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H7" t="s">
+        <v>255</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M7" s="1">
+        <f>IF(B7=B6,M6,M6+1)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <f>C8</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f>D8</f>
+        <v>20 Xbudget</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H8" t="s">
+        <v>256</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M8" s="1">
+        <f>IF(B8=B7,M7,M7+1)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f>C9</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>D9</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H9" t="s">
+        <v>244</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M9" s="1">
+        <f>IF(B9=B8,M8,M8+1)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f>C10</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>D10</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H10" t="s">
+        <v>245</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M10" s="1">
+        <f>IF(B10=B9,M9,M9+1)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f>C11</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>D11</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H11" t="s">
+        <v>237</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M11" s="1">
+        <f>IF(B11=B10,M10,M10+1)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f>C12</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>D12</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H12" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M12" s="1">
+        <f>IF(B12=B11,M11,M11+1)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f>C13</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>D13</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H13" t="s">
+        <v>246</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M13" s="1">
+        <f>IF(B13=B12,M12,M12+1)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f>C14</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>D14</f>
+        <v>Xbudget</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H14" t="s">
+        <v>247</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M14" s="1">
+        <f>IF(B14=B13,M13,M13+1)</f>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:M14">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD($M1,2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor update to small/large church entries
</commit_message>
<xml_diff>
--- a/input_files/map.xlsx
+++ b/input_files/map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\01_Dave\Programs\GitHub_home\budget\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\01_Dave\Programs\GitHub_home\budget\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA39FB4-C211-4DB9-830C-21DE0E131325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F370ABA-724C-4982-BE69-5889BAC4E5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10185" yWindow="0" windowWidth="18720" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -20,8 +20,8 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$244</definedName>
-    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable2" hidden="1">'[1]budget 11-01-23'!$A$1:$M$198</definedName>
-    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable3" hidden="1">Table1</definedName>
+    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable21" hidden="1">'[1]budget 11-01-23'!$A$1:$M$198</definedName>
+    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable31" hidden="1">Table1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -120,7 +120,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table2" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable2"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable21"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -129,7 +129,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table3">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable3"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable31"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2197" uniqueCount="350">
   <si>
     <t>Recurring or 1-time Expense</t>
   </si>
@@ -1563,9 +1563,9 @@
   <dimension ref="A1:L244"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L17" sqref="L17"/>
-      <selection pane="bottomLeft" activeCell="F155" sqref="F155"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1648,6 +1648,9 @@
       <c r="H2" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>206</v>
+      </c>
       <c r="K2" s="1" t="s">
         <v>249</v>
       </c>
@@ -1716,6 +1719,9 @@
       <c r="G4" t="s">
         <v>234</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>206</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>249</v>
       </c>
@@ -3187,6 +3193,9 @@
       <c r="G44" t="s">
         <v>240</v>
       </c>
+      <c r="J44" s="1" t="s">
+        <v>206</v>
+      </c>
       <c r="K44" s="1" t="s">
         <v>249</v>
       </c>
@@ -4859,7 +4868,7 @@
         <v>189</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K89" s="1" t="s">
         <v>4</v>
@@ -5564,6 +5573,9 @@
       <c r="G108" t="s">
         <v>231</v>
       </c>
+      <c r="J108" s="1" t="s">
+        <v>206</v>
+      </c>
       <c r="K108" s="1" t="s">
         <v>249</v>
       </c>
@@ -5743,6 +5755,9 @@
       <c r="G113" t="s">
         <v>241</v>
       </c>
+      <c r="J113" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K113" s="1" t="s">
         <v>249</v>
       </c>
@@ -8266,7 +8281,7 @@
         <v>189</v>
       </c>
       <c r="J181" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K181" s="1" t="s">
         <v>4</v>
@@ -10124,6 +10139,9 @@
       <c r="G231" t="s">
         <v>242</v>
       </c>
+      <c r="J231" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K231" s="1" t="s">
         <v>249</v>
       </c>
@@ -10155,6 +10173,9 @@
       <c r="G232" t="s">
         <v>233</v>
       </c>
+      <c r="J232" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K232" s="1" t="s">
         <v>249</v>
       </c>
@@ -10186,6 +10207,9 @@
       <c r="G233" t="s">
         <v>243</v>
       </c>
+      <c r="J233" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K233" s="1" t="s">
         <v>249</v>
       </c>
@@ -10217,6 +10241,9 @@
       <c r="G234" t="s">
         <v>244</v>
       </c>
+      <c r="J234" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K234" s="1" t="s">
         <v>249</v>
       </c>
@@ -10248,6 +10275,9 @@
       <c r="G235" t="s">
         <v>245</v>
       </c>
+      <c r="J235" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K235" s="1" t="s">
         <v>249</v>
       </c>
@@ -10279,6 +10309,9 @@
       <c r="G236" t="s">
         <v>246</v>
       </c>
+      <c r="J236" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K236" s="1" t="s">
         <v>249</v>
       </c>
@@ -10310,6 +10343,9 @@
       <c r="G237" t="s">
         <v>247</v>
       </c>
+      <c r="J237" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K237" s="1" t="s">
         <v>249</v>
       </c>
@@ -10341,6 +10377,9 @@
       <c r="G238" t="s">
         <v>248</v>
       </c>
+      <c r="J238" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K238" s="1" t="s">
         <v>249</v>
       </c>
@@ -10375,6 +10414,9 @@
       <c r="H239" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="J239" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K239" s="1" t="s">
         <v>249</v>
       </c>
@@ -10409,6 +10451,9 @@
       <c r="H240" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="J240" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K240" s="1" t="s">
         <v>249</v>
       </c>
@@ -10443,6 +10488,9 @@
       <c r="H241" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="J241" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K241" s="1" t="s">
         <v>249</v>
       </c>
@@ -10477,6 +10525,9 @@
       <c r="H242" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="J242" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K242" s="1" t="s">
         <v>249</v>
       </c>
@@ -10511,6 +10562,9 @@
       <c r="H243" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="J243" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="K243" s="1" t="s">
         <v>249</v>
       </c>
@@ -10544,6 +10598,9 @@
       </c>
       <c r="H244" s="1" t="s">
         <v>189</v>
+      </c>
+      <c r="J244" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="K244" s="1" t="s">
         <v>249</v>

</xml_diff>